<commit_message>
fix bit position for drilling operation. Update tests. Prepare new release: patch version 0.3.4
</commit_message>
<xml_diff>
--- a/pwptemp/tests/trajectory1.xlsx
+++ b/pwptemp/tests/trajectory1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanc/Library/Application Support/JetBrains/PyCharm2020.2/scratches/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanc/PycharmProjects/pwptemp/pwptemp/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9164C20-AE14-DF45-902E-FF6CC6DABAC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606540A3-DC2B-E847-946A-C06B739C685F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +72,12 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,11 +100,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -314,10 +321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X999"/>
+  <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -364,17 +371,17 @@
       <c r="X1" s="2"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>145.9</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="B2" s="4">
         <v>0</v>
       </c>
-      <c r="D2" s="3">
-        <v>145.9</v>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -399,7 +406,7 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>146</v>
+        <v>145.9</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -408,7 +415,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="3">
-        <v>146</v>
+        <v>145.9</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -433,16 +440,16 @@
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>154.9</v>
+        <v>146</v>
       </c>
       <c r="B4" s="3">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>221.03</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>154.9</v>
+        <v>146</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -467,16 +474,16 @@
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>195.3</v>
+        <v>154.9</v>
       </c>
       <c r="B5" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.16</v>
       </c>
       <c r="C5" s="3">
-        <v>98.15</v>
+        <v>221.03</v>
       </c>
       <c r="D5" s="3">
-        <v>195.3</v>
+        <v>154.9</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -501,16 +508,16 @@
     </row>
     <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>221</v>
+        <v>195.3</v>
       </c>
       <c r="B6" s="3">
-        <v>0.51</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C6" s="3">
-        <v>63.39</v>
+        <v>98.15</v>
       </c>
       <c r="D6" s="3">
-        <v>221</v>
+        <v>195.3</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -535,16 +542,16 @@
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>235.6</v>
+        <v>221</v>
       </c>
       <c r="B7" s="3">
-        <v>0.64</v>
+        <v>0.51</v>
       </c>
       <c r="C7" s="3">
-        <v>43.64</v>
+        <v>63.39</v>
       </c>
       <c r="D7" s="3">
-        <v>235.6</v>
+        <v>221</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -569,16 +576,16 @@
     </row>
     <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>276</v>
+        <v>235.6</v>
       </c>
       <c r="B8" s="3">
-        <v>1.51</v>
+        <v>0.64</v>
       </c>
       <c r="C8" s="3">
-        <v>188.03</v>
+        <v>43.64</v>
       </c>
       <c r="D8" s="3">
-        <v>276</v>
+        <v>235.6</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -603,16 +610,16 @@
     </row>
     <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>316.39999999999998</v>
+        <v>276</v>
       </c>
       <c r="B9" s="3">
-        <v>2.21</v>
+        <v>1.51</v>
       </c>
       <c r="C9" s="3">
-        <v>178.31</v>
+        <v>188.03</v>
       </c>
       <c r="D9" s="3">
-        <v>316.39999999999998</v>
+        <v>276</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -637,16 +644,16 @@
     </row>
     <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>356.7</v>
+        <v>316.39999999999998</v>
       </c>
       <c r="B10" s="3">
-        <v>4.1100000000000003</v>
+        <v>2.21</v>
       </c>
       <c r="C10" s="3">
-        <v>173.29</v>
+        <v>178.31</v>
       </c>
       <c r="D10" s="3">
-        <v>356.6</v>
+        <v>316.39999999999998</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -671,16 +678,16 @@
     </row>
     <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>397.1</v>
+        <v>356.7</v>
       </c>
       <c r="B11" s="3">
-        <v>7.66</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="C11" s="3">
-        <v>171.91</v>
+        <v>173.29</v>
       </c>
       <c r="D11" s="3">
-        <v>396.8</v>
+        <v>356.6</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -705,16 +712,16 @@
     </row>
     <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>437.5</v>
+        <v>397.1</v>
       </c>
       <c r="B12" s="3">
-        <v>9.1300000000000008</v>
+        <v>7.66</v>
       </c>
       <c r="C12" s="3">
-        <v>178.88</v>
+        <v>171.91</v>
       </c>
       <c r="D12" s="3">
-        <v>436.8</v>
+        <v>396.8</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -739,16 +746,16 @@
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>477.8</v>
+        <v>437.5</v>
       </c>
       <c r="B13" s="3">
-        <v>10.58</v>
+        <v>9.1300000000000008</v>
       </c>
       <c r="C13" s="3">
-        <v>180.1</v>
+        <v>178.88</v>
       </c>
       <c r="D13" s="3">
-        <v>476.5</v>
+        <v>436.8</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -773,16 +780,16 @@
     </row>
     <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>518.20000000000005</v>
+        <v>477.8</v>
       </c>
       <c r="B14" s="3">
-        <v>11.35</v>
+        <v>10.58</v>
       </c>
       <c r="C14" s="3">
-        <v>177.18</v>
+        <v>180.1</v>
       </c>
       <c r="D14" s="3">
-        <v>516.1</v>
+        <v>476.5</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -807,16 +814,16 @@
     </row>
     <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>558.5</v>
+        <v>518.20000000000005</v>
       </c>
       <c r="B15" s="3">
-        <v>11.51</v>
+        <v>11.35</v>
       </c>
       <c r="C15" s="3">
-        <v>168.58</v>
+        <v>177.18</v>
       </c>
       <c r="D15" s="3">
-        <v>555.6</v>
+        <v>516.1</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -841,16 +848,16 @@
     </row>
     <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>598.9</v>
+        <v>558.5</v>
       </c>
       <c r="B16" s="3">
-        <v>12.38</v>
+        <v>11.51</v>
       </c>
       <c r="C16" s="3">
-        <v>160.99</v>
+        <v>168.58</v>
       </c>
       <c r="D16" s="3">
-        <v>595.20000000000005</v>
+        <v>555.6</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -875,16 +882,16 @@
     </row>
     <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>639.29999999999995</v>
+        <v>598.9</v>
       </c>
       <c r="B17" s="3">
-        <v>13.56</v>
+        <v>12.38</v>
       </c>
       <c r="C17" s="3">
-        <v>152.13999999999999</v>
+        <v>160.99</v>
       </c>
       <c r="D17" s="3">
-        <v>634.5</v>
+        <v>595.20000000000005</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -909,16 +916,16 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>679.6</v>
+        <v>639.29999999999995</v>
       </c>
       <c r="B18" s="3">
-        <v>14.3</v>
+        <v>13.56</v>
       </c>
       <c r="C18" s="3">
-        <v>144.13999999999999</v>
+        <v>152.13999999999999</v>
       </c>
       <c r="D18" s="3">
-        <v>673.7</v>
+        <v>634.5</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -943,16 +950,16 @@
     </row>
     <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>720</v>
+        <v>679.6</v>
       </c>
       <c r="B19" s="3">
-        <v>15.63</v>
+        <v>14.3</v>
       </c>
       <c r="C19" s="3">
-        <v>138.03</v>
+        <v>144.13999999999999</v>
       </c>
       <c r="D19" s="3">
-        <v>712.7</v>
+        <v>673.7</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -977,16 +984,16 @@
     </row>
     <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>760.4</v>
+        <v>720</v>
       </c>
       <c r="B20" s="3">
-        <v>18.5</v>
+        <v>15.63</v>
       </c>
       <c r="C20" s="3">
-        <v>128.65</v>
+        <v>138.03</v>
       </c>
       <c r="D20" s="3">
-        <v>751.3</v>
+        <v>712.7</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1011,16 +1018,16 @@
     </row>
     <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>800.7</v>
+        <v>760.4</v>
       </c>
       <c r="B21" s="3">
-        <v>21.63</v>
+        <v>18.5</v>
       </c>
       <c r="C21" s="3">
-        <v>122.01</v>
+        <v>128.65</v>
       </c>
       <c r="D21" s="3">
-        <v>789.2</v>
+        <v>751.3</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1045,16 +1052,16 @@
     </row>
     <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>841.1</v>
+        <v>800.7</v>
       </c>
       <c r="B22" s="3">
-        <v>23.86</v>
+        <v>21.63</v>
       </c>
       <c r="C22" s="3">
-        <v>117.08</v>
+        <v>122.01</v>
       </c>
       <c r="D22" s="3">
-        <v>826.4</v>
+        <v>789.2</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1079,16 +1086,16 @@
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>881.5</v>
+        <v>841.1</v>
       </c>
       <c r="B23" s="3">
-        <v>26.84</v>
+        <v>23.86</v>
       </c>
       <c r="C23" s="3">
-        <v>113.98</v>
+        <v>117.08</v>
       </c>
       <c r="D23" s="3">
-        <v>862.9</v>
+        <v>826.4</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -1113,16 +1120,16 @@
     </row>
     <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>921.8</v>
+        <v>881.5</v>
       </c>
       <c r="B24" s="3">
-        <v>25.33</v>
+        <v>26.84</v>
       </c>
       <c r="C24" s="3">
-        <v>116.92</v>
+        <v>113.98</v>
       </c>
       <c r="D24" s="3">
-        <v>899.1</v>
+        <v>862.9</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1147,16 +1154,16 @@
     </row>
     <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>962.2</v>
+        <v>921.8</v>
       </c>
       <c r="B25" s="3">
-        <v>22.47</v>
+        <v>25.33</v>
       </c>
       <c r="C25" s="3">
-        <v>119.01</v>
+        <v>116.92</v>
       </c>
       <c r="D25" s="3">
-        <v>936.1</v>
+        <v>899.1</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -1181,16 +1188,16 @@
     </row>
     <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>1002.6</v>
+        <v>962.2</v>
       </c>
       <c r="B26" s="3">
-        <v>19.82</v>
+        <v>22.47</v>
       </c>
       <c r="C26" s="3">
-        <v>122.15</v>
+        <v>119.01</v>
       </c>
       <c r="D26" s="3">
-        <v>973.7</v>
+        <v>936.1</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -1215,16 +1222,16 @@
     </row>
     <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>1043</v>
+        <v>1002.6</v>
       </c>
       <c r="B27" s="3">
-        <v>17.2</v>
+        <v>19.82</v>
       </c>
       <c r="C27" s="3">
-        <v>122.87</v>
+        <v>122.15</v>
       </c>
       <c r="D27" s="3">
-        <v>1012</v>
+        <v>973.7</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -1249,16 +1256,16 @@
     </row>
     <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>1083.3</v>
+        <v>1043</v>
       </c>
       <c r="B28" s="3">
-        <v>15</v>
+        <v>17.2</v>
       </c>
       <c r="C28" s="3">
-        <v>123.11</v>
+        <v>122.87</v>
       </c>
       <c r="D28" s="3">
-        <v>1050.8</v>
+        <v>1012</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1283,16 +1290,16 @@
     </row>
     <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>1123.7</v>
+        <v>1083.3</v>
       </c>
       <c r="B29" s="3">
-        <v>17.73</v>
+        <v>15</v>
       </c>
       <c r="C29" s="3">
-        <v>118.94</v>
+        <v>123.11</v>
       </c>
       <c r="D29" s="3">
-        <v>1089.5</v>
+        <v>1050.8</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -1317,16 +1324,16 @@
     </row>
     <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>1164.0999999999999</v>
+        <v>1123.7</v>
       </c>
       <c r="B30" s="3">
-        <v>21.77</v>
+        <v>17.73</v>
       </c>
       <c r="C30" s="3">
-        <v>113.96</v>
+        <v>118.94</v>
       </c>
       <c r="D30" s="3">
-        <v>1127.5</v>
+        <v>1089.5</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1351,16 +1358,16 @@
     </row>
     <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>1204.4000000000001</v>
+        <v>1164.0999999999999</v>
       </c>
       <c r="B31" s="3">
-        <v>26.13</v>
+        <v>21.77</v>
       </c>
       <c r="C31" s="3">
-        <v>110.24</v>
+        <v>113.96</v>
       </c>
       <c r="D31" s="3">
-        <v>1164.4000000000001</v>
+        <v>1127.5</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -1385,16 +1392,16 @@
     </row>
     <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>1244.8</v>
+        <v>1204.4000000000001</v>
       </c>
       <c r="B32" s="3">
-        <v>29.6</v>
+        <v>26.13</v>
       </c>
       <c r="C32" s="3">
-        <v>108.19</v>
+        <v>110.24</v>
       </c>
       <c r="D32" s="3">
-        <v>1200.0999999999999</v>
+        <v>1164.4000000000001</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -1419,16 +1426,16 @@
     </row>
     <row r="33" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>1285.2</v>
+        <v>1244.8</v>
       </c>
       <c r="B33" s="3">
-        <v>31.04</v>
+        <v>29.6</v>
       </c>
       <c r="C33" s="3">
-        <v>109.95</v>
+        <v>108.19</v>
       </c>
       <c r="D33" s="3">
-        <v>1234.9000000000001</v>
+        <v>1200.0999999999999</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -1453,16 +1460,16 @@
     </row>
     <row r="34" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>1325.6</v>
+        <v>1285.2</v>
       </c>
       <c r="B34" s="3">
-        <v>28.6</v>
+        <v>31.04</v>
       </c>
       <c r="C34" s="3">
-        <v>112.14</v>
+        <v>109.95</v>
       </c>
       <c r="D34" s="3">
-        <v>1270</v>
+        <v>1234.9000000000001</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -1487,16 +1494,16 @@
     </row>
     <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>1365.9</v>
+        <v>1325.6</v>
       </c>
       <c r="B35" s="3">
-        <v>25.5</v>
+        <v>28.6</v>
       </c>
       <c r="C35" s="3">
-        <v>114.9</v>
+        <v>112.14</v>
       </c>
       <c r="D35" s="3">
-        <v>1305.9000000000001</v>
+        <v>1270</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -1521,16 +1528,16 @@
     </row>
     <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>1405</v>
+        <v>1365.9</v>
       </c>
       <c r="B36" s="3">
-        <v>29.75</v>
+        <v>25.5</v>
       </c>
       <c r="C36" s="3">
-        <v>114.66</v>
+        <v>114.9</v>
       </c>
       <c r="D36" s="3">
-        <v>1340.5</v>
+        <v>1305.9000000000001</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1555,16 +1562,16 @@
     </row>
     <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>1406.3</v>
+        <v>1405</v>
       </c>
       <c r="B37" s="3">
-        <v>29.89</v>
+        <v>29.75</v>
       </c>
       <c r="C37" s="3">
-        <v>114.65</v>
+        <v>114.66</v>
       </c>
       <c r="D37" s="3">
-        <v>1341.6</v>
+        <v>1340.5</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -1589,16 +1596,16 @@
     </row>
     <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>1446.6</v>
+        <v>1406.3</v>
       </c>
       <c r="B38" s="3">
-        <v>31.1</v>
+        <v>29.89</v>
       </c>
       <c r="C38" s="3">
-        <v>113.78</v>
+        <v>114.65</v>
       </c>
       <c r="D38" s="3">
-        <v>1376.4</v>
+        <v>1341.6</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -1623,16 +1630,16 @@
     </row>
     <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>1487</v>
+        <v>1446.6</v>
       </c>
       <c r="B39" s="3">
-        <v>31.91</v>
+        <v>31.1</v>
       </c>
       <c r="C39" s="3">
-        <v>113.02</v>
+        <v>113.78</v>
       </c>
       <c r="D39" s="3">
-        <v>1410.8</v>
+        <v>1376.4</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -1657,16 +1664,16 @@
     </row>
     <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>1527.3</v>
+        <v>1487</v>
       </c>
       <c r="B40" s="3">
-        <v>31.93</v>
+        <v>31.91</v>
       </c>
       <c r="C40" s="3">
         <v>113.02</v>
       </c>
       <c r="D40" s="3">
-        <v>1445</v>
+        <v>1410.8</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -1691,16 +1698,16 @@
     </row>
     <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>1567.7</v>
+        <v>1527.3</v>
       </c>
       <c r="B41" s="3">
-        <v>32.67</v>
+        <v>31.93</v>
       </c>
       <c r="C41" s="3">
-        <v>110.91</v>
+        <v>113.02</v>
       </c>
       <c r="D41" s="3">
-        <v>1479.2</v>
+        <v>1445</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -1725,16 +1732,16 @@
     </row>
     <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>1608</v>
+        <v>1567.7</v>
       </c>
       <c r="B42" s="3">
-        <v>33.69</v>
+        <v>32.67</v>
       </c>
       <c r="C42" s="3">
-        <v>107.7</v>
+        <v>110.91</v>
       </c>
       <c r="D42" s="3">
-        <v>1512.9</v>
+        <v>1479.2</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -1759,16 +1766,16 @@
     </row>
     <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>1648.4</v>
+        <v>1608</v>
       </c>
       <c r="B43" s="3">
-        <v>34.24</v>
+        <v>33.69</v>
       </c>
       <c r="C43" s="3">
-        <v>106.15</v>
+        <v>107.7</v>
       </c>
       <c r="D43" s="3">
-        <v>1546.4</v>
+        <v>1512.9</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -1793,16 +1800,16 @@
     </row>
     <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>1688.8</v>
+        <v>1648.4</v>
       </c>
       <c r="B44" s="3">
-        <v>34.99</v>
+        <v>34.24</v>
       </c>
       <c r="C44" s="3">
-        <v>103.16</v>
+        <v>106.15</v>
       </c>
       <c r="D44" s="3">
-        <v>1579.7</v>
+        <v>1546.4</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -1827,16 +1834,16 @@
     </row>
     <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>1729.1</v>
+        <v>1688.8</v>
       </c>
       <c r="B45" s="3">
-        <v>35.880000000000003</v>
+        <v>34.99</v>
       </c>
       <c r="C45" s="3">
-        <v>101.36</v>
+        <v>103.16</v>
       </c>
       <c r="D45" s="3">
-        <v>1612.5</v>
+        <v>1579.7</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
@@ -1861,16 +1868,16 @@
     </row>
     <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>1769.5</v>
+        <v>1729.1</v>
       </c>
       <c r="B46" s="3">
-        <v>35.93</v>
+        <v>35.880000000000003</v>
       </c>
       <c r="C46" s="3">
-        <v>103.37</v>
+        <v>101.36</v>
       </c>
       <c r="D46" s="3">
-        <v>1645.2</v>
+        <v>1612.5</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -1895,16 +1902,16 @@
     </row>
     <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>1809.8</v>
+        <v>1769.5</v>
       </c>
       <c r="B47" s="3">
-        <v>35.950000000000003</v>
+        <v>35.93</v>
       </c>
       <c r="C47" s="3">
-        <v>104.77</v>
+        <v>103.37</v>
       </c>
       <c r="D47" s="3">
-        <v>1677.9</v>
+        <v>1645.2</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
@@ -1929,16 +1936,16 @@
     </row>
     <row r="48" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>1850.2</v>
+        <v>1809.8</v>
       </c>
       <c r="B48" s="3">
-        <v>35.83</v>
+        <v>35.950000000000003</v>
       </c>
       <c r="C48" s="3">
-        <v>106.25</v>
+        <v>104.77</v>
       </c>
       <c r="D48" s="3">
-        <v>1710.6</v>
+        <v>1677.9</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
@@ -1963,16 +1970,16 @@
     </row>
     <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>1890.6</v>
+        <v>1850.2</v>
       </c>
       <c r="B49" s="3">
-        <v>36.049999999999997</v>
+        <v>35.83</v>
       </c>
       <c r="C49" s="3">
-        <v>109.56</v>
+        <v>106.25</v>
       </c>
       <c r="D49" s="3">
-        <v>1743.3</v>
+        <v>1710.6</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -1997,16 +2004,16 @@
     </row>
     <row r="50" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>1930.9</v>
+        <v>1890.6</v>
       </c>
       <c r="B50" s="3">
-        <v>36.799999999999997</v>
+        <v>36.049999999999997</v>
       </c>
       <c r="C50" s="3">
-        <v>111.45</v>
+        <v>109.56</v>
       </c>
       <c r="D50" s="3">
-        <v>1775.7</v>
+        <v>1743.3</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -2031,16 +2038,16 @@
     </row>
     <row r="51" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>1971.3</v>
+        <v>1930.9</v>
       </c>
       <c r="B51" s="3">
-        <v>36.159999999999997</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="C51" s="3">
-        <v>113.43</v>
+        <v>111.45</v>
       </c>
       <c r="D51" s="3">
-        <v>1808.2</v>
+        <v>1775.7</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
@@ -2065,16 +2072,16 @@
     </row>
     <row r="52" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>2011.7</v>
+        <v>1971.3</v>
       </c>
       <c r="B52" s="3">
-        <v>35.9</v>
+        <v>36.159999999999997</v>
       </c>
       <c r="C52" s="3">
-        <v>113.73</v>
+        <v>113.43</v>
       </c>
       <c r="D52" s="3">
-        <v>1840.9</v>
+        <v>1808.2</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
@@ -2099,16 +2106,16 @@
     </row>
     <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <v>2052</v>
+        <v>2011.7</v>
       </c>
       <c r="B53" s="3">
-        <v>34.880000000000003</v>
+        <v>35.9</v>
       </c>
       <c r="C53" s="3">
-        <v>114.41</v>
+        <v>113.73</v>
       </c>
       <c r="D53" s="3">
-        <v>1873.7</v>
+        <v>1840.9</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
@@ -2133,16 +2140,16 @@
     </row>
     <row r="54" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>2092.4</v>
+        <v>2052</v>
       </c>
       <c r="B54" s="3">
-        <v>33.5</v>
+        <v>34.880000000000003</v>
       </c>
       <c r="C54" s="3">
-        <v>112.95</v>
+        <v>114.41</v>
       </c>
       <c r="D54" s="3">
-        <v>1907.1</v>
+        <v>1873.7</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
@@ -2167,16 +2174,16 @@
     </row>
     <row r="55" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>2132.6999999999998</v>
+        <v>2092.4</v>
       </c>
       <c r="B55" s="3">
-        <v>32.25</v>
+        <v>33.5</v>
       </c>
       <c r="C55" s="3">
-        <v>110.97</v>
+        <v>112.95</v>
       </c>
       <c r="D55" s="3">
-        <v>1941</v>
+        <v>1907.1</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
@@ -2201,16 +2208,16 @@
     </row>
     <row r="56" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>2173</v>
+        <v>2132.6999999999998</v>
       </c>
       <c r="B56" s="3">
-        <v>32.85</v>
+        <v>32.25</v>
       </c>
       <c r="C56" s="3">
-        <v>108.23</v>
+        <v>110.97</v>
       </c>
       <c r="D56" s="3">
-        <v>1975</v>
+        <v>1941</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
@@ -2235,16 +2242,16 @@
     </row>
     <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>2213.4</v>
+        <v>2173</v>
       </c>
       <c r="B57" s="3">
-        <v>32.96</v>
+        <v>32.85</v>
       </c>
       <c r="C57" s="3">
-        <v>103.95</v>
+        <v>108.23</v>
       </c>
       <c r="D57" s="3">
-        <v>2008.9</v>
+        <v>1975</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
@@ -2269,16 +2276,16 @@
     </row>
     <row r="58" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>2253.6999999999998</v>
+        <v>2213.4</v>
       </c>
       <c r="B58" s="3">
-        <v>33.130000000000003</v>
+        <v>32.96</v>
       </c>
       <c r="C58" s="3">
-        <v>101.52</v>
+        <v>103.95</v>
       </c>
       <c r="D58" s="3">
-        <v>2042.7</v>
+        <v>2008.9</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
@@ -2303,16 +2310,16 @@
     </row>
     <row r="59" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <v>2294.1</v>
+        <v>2253.6999999999998</v>
       </c>
       <c r="B59" s="3">
-        <v>33.06</v>
+        <v>33.130000000000003</v>
       </c>
       <c r="C59" s="3">
-        <v>98.75</v>
+        <v>101.52</v>
       </c>
       <c r="D59" s="3">
-        <v>2076.5</v>
+        <v>2042.7</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
@@ -2337,16 +2344,16 @@
     </row>
     <row r="60" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <v>2334.4</v>
+        <v>2294.1</v>
       </c>
       <c r="B60" s="3">
-        <v>33.270000000000003</v>
+        <v>33.06</v>
       </c>
       <c r="C60" s="3">
-        <v>95.46</v>
+        <v>98.75</v>
       </c>
       <c r="D60" s="3">
-        <v>2110.3000000000002</v>
+        <v>2076.5</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
@@ -2371,16 +2378,16 @@
     </row>
     <row r="61" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>2374.8000000000002</v>
+        <v>2334.4</v>
       </c>
       <c r="B61" s="3">
-        <v>33.479999999999997</v>
+        <v>33.270000000000003</v>
       </c>
       <c r="C61" s="3">
-        <v>93.92</v>
+        <v>95.46</v>
       </c>
       <c r="D61" s="3">
-        <v>2144</v>
+        <v>2110.3000000000002</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
@@ -2405,16 +2412,16 @@
     </row>
     <row r="62" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>2415.1999999999998</v>
+        <v>2374.8000000000002</v>
       </c>
       <c r="B62" s="3">
-        <v>33.450000000000003</v>
+        <v>33.479999999999997</v>
       </c>
       <c r="C62" s="3">
-        <v>93.04</v>
+        <v>93.92</v>
       </c>
       <c r="D62" s="3">
-        <v>2177.6999999999998</v>
+        <v>2144</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
@@ -2439,16 +2446,16 @@
     </row>
     <row r="63" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
-        <v>2455.6</v>
+        <v>2415.1999999999998</v>
       </c>
       <c r="B63" s="3">
-        <v>33.33</v>
+        <v>33.450000000000003</v>
       </c>
       <c r="C63" s="3">
-        <v>91.93</v>
+        <v>93.04</v>
       </c>
       <c r="D63" s="3">
-        <v>2211.4</v>
+        <v>2177.6999999999998</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
@@ -2473,16 +2480,16 @@
     </row>
     <row r="64" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <v>2496</v>
+        <v>2455.6</v>
       </c>
       <c r="B64" s="3">
-        <v>32.61</v>
+        <v>33.33</v>
       </c>
       <c r="C64" s="3">
-        <v>92.01</v>
+        <v>91.93</v>
       </c>
       <c r="D64" s="3">
-        <v>2245.3000000000002</v>
+        <v>2211.4</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
@@ -2507,16 +2514,16 @@
     </row>
     <row r="65" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
-        <v>2536.3000000000002</v>
+        <v>2496</v>
       </c>
       <c r="B65" s="3">
-        <v>31.9</v>
+        <v>32.61</v>
       </c>
       <c r="C65" s="3">
-        <v>90.38</v>
+        <v>92.01</v>
       </c>
       <c r="D65" s="3">
-        <v>2279.4</v>
+        <v>2245.3000000000002</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
@@ -2541,16 +2548,16 @@
     </row>
     <row r="66" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
-        <v>2576.6999999999998</v>
+        <v>2536.3000000000002</v>
       </c>
       <c r="B66" s="3">
-        <v>31.49</v>
+        <v>31.9</v>
       </c>
       <c r="C66" s="3">
-        <v>87.08</v>
+        <v>90.38</v>
       </c>
       <c r="D66" s="3">
-        <v>2313.8000000000002</v>
+        <v>2279.4</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
@@ -2575,16 +2582,16 @@
     </row>
     <row r="67" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
-        <v>2617.1</v>
+        <v>2576.6999999999998</v>
       </c>
       <c r="B67" s="3">
-        <v>31.21</v>
+        <v>31.49</v>
       </c>
       <c r="C67" s="3">
-        <v>84.61</v>
+        <v>87.08</v>
       </c>
       <c r="D67" s="3">
-        <v>2348.3000000000002</v>
+        <v>2313.8000000000002</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
@@ -2609,16 +2616,16 @@
     </row>
     <row r="68" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <v>2657.4</v>
+        <v>2617.1</v>
       </c>
       <c r="B68" s="3">
-        <v>31.29</v>
+        <v>31.21</v>
       </c>
       <c r="C68" s="3">
-        <v>83.98</v>
+        <v>84.61</v>
       </c>
       <c r="D68" s="3">
-        <v>2382.6999999999998</v>
+        <v>2348.3000000000002</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
@@ -2643,16 +2650,16 @@
     </row>
     <row r="69" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <v>2697.8</v>
+        <v>2657.4</v>
       </c>
       <c r="B69" s="3">
-        <v>31.42</v>
+        <v>31.29</v>
       </c>
       <c r="C69" s="3">
-        <v>85.86</v>
+        <v>83.98</v>
       </c>
       <c r="D69" s="3">
-        <v>2417.1999999999998</v>
+        <v>2382.6999999999998</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -2677,16 +2684,16 @@
     </row>
     <row r="70" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <v>2738.2</v>
+        <v>2697.8</v>
       </c>
       <c r="B70" s="3">
-        <v>31.03</v>
+        <v>31.42</v>
       </c>
       <c r="C70" s="3">
-        <v>84.46</v>
+        <v>85.86</v>
       </c>
       <c r="D70" s="3">
-        <v>2451.8000000000002</v>
+        <v>2417.1999999999998</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
@@ -2711,16 +2718,16 @@
     </row>
     <row r="71" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
-        <v>2775.5</v>
+        <v>2738.2</v>
       </c>
       <c r="B71" s="3">
-        <v>30.68</v>
+        <v>31.03</v>
       </c>
       <c r="C71" s="3">
-        <v>81.14</v>
+        <v>84.46</v>
       </c>
       <c r="D71" s="3">
-        <v>2483.8000000000002</v>
+        <v>2451.8000000000002</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -2745,16 +2752,16 @@
     </row>
     <row r="72" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
-        <v>2789.4</v>
+        <v>2775.5</v>
       </c>
       <c r="B72" s="3">
-        <v>30.65</v>
+        <v>30.68</v>
       </c>
       <c r="C72" s="3">
-        <v>80.78</v>
+        <v>81.14</v>
       </c>
       <c r="D72" s="3">
-        <v>2495.8000000000002</v>
+        <v>2483.8000000000002</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
@@ -2779,16 +2786,16 @@
     </row>
     <row r="73" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
-        <v>2829.6</v>
+        <v>2789.4</v>
       </c>
       <c r="B73" s="3">
-        <v>30.89</v>
+        <v>30.65</v>
       </c>
       <c r="C73" s="3">
-        <v>78.69</v>
+        <v>80.78</v>
       </c>
       <c r="D73" s="3">
-        <v>2530.3000000000002</v>
+        <v>2495.8000000000002</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -2813,16 +2820,16 @@
     </row>
     <row r="74" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
-        <v>2866.9</v>
+        <v>2829.6</v>
       </c>
       <c r="B74" s="3">
-        <v>30.86</v>
+        <v>30.89</v>
       </c>
       <c r="C74" s="3">
-        <v>77.5</v>
+        <v>78.69</v>
       </c>
       <c r="D74" s="3">
-        <v>2562.3000000000002</v>
+        <v>2530.3000000000002</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -2847,16 +2854,16 @@
     </row>
     <row r="75" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
-        <v>2904.4</v>
+        <v>2866.9</v>
       </c>
       <c r="B75" s="3">
-        <v>31.2</v>
+        <v>30.86</v>
       </c>
       <c r="C75" s="3">
-        <v>77.010000000000005</v>
+        <v>77.5</v>
       </c>
       <c r="D75" s="3">
-        <v>2594.5</v>
+        <v>2562.3000000000002</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -2881,16 +2888,16 @@
     </row>
     <row r="76" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
-        <v>2913.3</v>
+        <v>2904.4</v>
       </c>
       <c r="B76" s="3">
-        <v>31.86</v>
+        <v>31.2</v>
       </c>
       <c r="C76" s="3">
-        <v>76.7</v>
+        <v>77.010000000000005</v>
       </c>
       <c r="D76" s="3">
-        <v>2602.1</v>
+        <v>2594.5</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
@@ -2915,16 +2922,16 @@
     </row>
     <row r="77" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <v>2921</v>
+        <v>2913.3</v>
       </c>
       <c r="B77" s="3">
-        <v>32.14</v>
+        <v>31.86</v>
       </c>
       <c r="C77" s="3">
-        <v>76.569999999999993</v>
+        <v>76.7</v>
       </c>
       <c r="D77" s="3">
-        <v>2608.6</v>
+        <v>2602.1</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -2949,16 +2956,16 @@
     </row>
     <row r="78" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <v>2927.7</v>
+        <v>2921</v>
       </c>
       <c r="B78" s="3">
-        <v>32.380000000000003</v>
+        <v>32.14</v>
       </c>
       <c r="C78" s="3">
-        <v>76.45</v>
+        <v>76.569999999999993</v>
       </c>
       <c r="D78" s="3">
-        <v>2614.1999999999998</v>
+        <v>2608.6</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
@@ -2983,16 +2990,16 @@
     </row>
     <row r="79" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
-        <v>2954.6</v>
+        <v>2927.7</v>
       </c>
       <c r="B79" s="3">
-        <v>34.03</v>
+        <v>32.380000000000003</v>
       </c>
       <c r="C79" s="3">
-        <v>71.62</v>
+        <v>76.45</v>
       </c>
       <c r="D79" s="3">
-        <v>2636.7</v>
+        <v>2614.1999999999998</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
@@ -3017,16 +3024,16 @@
     </row>
     <row r="80" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
-        <v>2995.2</v>
+        <v>2954.6</v>
       </c>
       <c r="B80" s="3">
-        <v>36.51</v>
+        <v>34.03</v>
       </c>
       <c r="C80" s="3">
-        <v>61.44</v>
+        <v>71.62</v>
       </c>
       <c r="D80" s="3">
-        <v>2669.9</v>
+        <v>2636.7</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
@@ -3051,16 +3058,16 @@
     </row>
     <row r="81" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
-        <v>3036.4</v>
+        <v>2995.2</v>
       </c>
       <c r="B81" s="3">
-        <v>36.770000000000003</v>
+        <v>36.51</v>
       </c>
       <c r="C81" s="3">
-        <v>55.01</v>
+        <v>61.44</v>
       </c>
       <c r="D81" s="3">
-        <v>2703</v>
+        <v>2669.9</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
@@ -3085,16 +3092,16 @@
     </row>
     <row r="82" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
-        <v>3076.7</v>
+        <v>3036.4</v>
       </c>
       <c r="B82" s="3">
-        <v>37.729999999999997</v>
+        <v>36.770000000000003</v>
       </c>
       <c r="C82" s="3">
-        <v>48.33</v>
+        <v>55.01</v>
       </c>
       <c r="D82" s="3">
-        <v>2735.1</v>
+        <v>2703</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
@@ -3119,16 +3126,16 @@
     </row>
     <row r="83" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
-        <v>3117.2</v>
+        <v>3076.7</v>
       </c>
       <c r="B83" s="3">
-        <v>37.11</v>
+        <v>37.729999999999997</v>
       </c>
       <c r="C83" s="3">
-        <v>43.61</v>
+        <v>48.33</v>
       </c>
       <c r="D83" s="3">
-        <v>2767.2</v>
+        <v>2735.1</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
@@ -3153,16 +3160,16 @@
     </row>
     <row r="84" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
-        <v>3157.5</v>
+        <v>3117.2</v>
       </c>
       <c r="B84" s="3">
-        <v>35.729999999999997</v>
+        <v>37.11</v>
       </c>
       <c r="C84" s="3">
-        <v>34.79</v>
+        <v>43.61</v>
       </c>
       <c r="D84" s="3">
-        <v>2799.7</v>
+        <v>2767.2</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
@@ -3187,16 +3194,16 @@
     </row>
     <row r="85" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
-        <v>3197</v>
+        <v>3157.5</v>
       </c>
       <c r="B85" s="3">
-        <v>34.200000000000003</v>
+        <v>35.729999999999997</v>
       </c>
       <c r="C85" s="3">
-        <v>28.91</v>
+        <v>34.79</v>
       </c>
       <c r="D85" s="3">
-        <v>2832.1</v>
+        <v>2799.7</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
@@ -3221,16 +3228,16 @@
     </row>
     <row r="86" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
-        <v>3236.9</v>
+        <v>3197</v>
       </c>
       <c r="B86" s="3">
-        <v>31.59</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="C86" s="3">
-        <v>21.36</v>
+        <v>28.91</v>
       </c>
       <c r="D86" s="3">
-        <v>2865.6</v>
+        <v>2832.1</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
@@ -3255,16 +3262,16 @@
     </row>
     <row r="87" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
-        <v>3253.8</v>
+        <v>3236.9</v>
       </c>
       <c r="B87" s="3">
-        <v>30.18</v>
+        <v>31.59</v>
       </c>
       <c r="C87" s="3">
-        <v>19.04</v>
+        <v>21.36</v>
       </c>
       <c r="D87" s="3">
-        <v>2880.1</v>
+        <v>2865.6</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
@@ -3289,16 +3296,16 @@
     </row>
     <row r="88" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
-        <v>3278.3</v>
+        <v>3253.8</v>
       </c>
       <c r="B88" s="3">
-        <v>28.32</v>
+        <v>30.18</v>
       </c>
       <c r="C88" s="3">
-        <v>16.57</v>
+        <v>19.04</v>
       </c>
       <c r="D88" s="3">
-        <v>2901.5</v>
+        <v>2880.1</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
@@ -3323,16 +3330,16 @@
     </row>
     <row r="89" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
-        <v>3319</v>
+        <v>3278.3</v>
       </c>
       <c r="B89" s="3">
-        <v>30.91</v>
+        <v>28.32</v>
       </c>
       <c r="C89" s="3">
-        <v>22.37</v>
+        <v>16.57</v>
       </c>
       <c r="D89" s="3">
-        <v>2936.9</v>
+        <v>2901.5</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
@@ -3357,16 +3364,16 @@
     </row>
     <row r="90" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
-        <v>3359.2</v>
+        <v>3319</v>
       </c>
       <c r="B90" s="3">
-        <v>34.92</v>
+        <v>30.91</v>
       </c>
       <c r="C90" s="3">
-        <v>27.52</v>
+        <v>22.37</v>
       </c>
       <c r="D90" s="3">
-        <v>2970.6</v>
+        <v>2936.9</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
@@ -3391,16 +3398,16 @@
     </row>
     <row r="91" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
-        <v>3398.5</v>
+        <v>3359.2</v>
       </c>
       <c r="B91" s="3">
-        <v>40.44</v>
+        <v>34.92</v>
       </c>
       <c r="C91" s="3">
-        <v>30.9</v>
+        <v>27.52</v>
       </c>
       <c r="D91" s="3">
-        <v>3001.7</v>
+        <v>2970.6</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
@@ -3425,16 +3432,16 @@
     </row>
     <row r="92" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <v>3439.6</v>
+        <v>3398.5</v>
       </c>
       <c r="B92" s="3">
-        <v>44.73</v>
+        <v>40.44</v>
       </c>
       <c r="C92" s="3">
-        <v>31.42</v>
+        <v>30.9</v>
       </c>
       <c r="D92" s="3">
-        <v>3031.9</v>
+        <v>3001.7</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
@@ -3459,16 +3466,16 @@
     </row>
     <row r="93" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <v>3479.3</v>
+        <v>3439.6</v>
       </c>
       <c r="B93" s="3">
-        <v>47.93</v>
+        <v>44.73</v>
       </c>
       <c r="C93" s="3">
-        <v>28.18</v>
+        <v>31.42</v>
       </c>
       <c r="D93" s="3">
-        <v>3059.4</v>
+        <v>3031.9</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
@@ -3493,16 +3500,16 @@
     </row>
     <row r="94" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
-        <v>3520.4</v>
+        <v>3479.3</v>
       </c>
       <c r="B94" s="3">
-        <v>50.65</v>
+        <v>47.93</v>
       </c>
       <c r="C94" s="3">
-        <v>26.17</v>
+        <v>28.18</v>
       </c>
       <c r="D94" s="3">
-        <v>3086.1</v>
+        <v>3059.4</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
@@ -3527,16 +3534,16 @@
     </row>
     <row r="95" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
-        <v>3559.9</v>
+        <v>3520.4</v>
       </c>
       <c r="B95" s="3">
-        <v>53.98</v>
+        <v>50.65</v>
       </c>
       <c r="C95" s="3">
-        <v>23.14</v>
+        <v>26.17</v>
       </c>
       <c r="D95" s="3">
-        <v>3110.3</v>
+        <v>3086.1</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
@@ -3561,16 +3568,16 @@
     </row>
     <row r="96" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
-        <v>3601.7</v>
+        <v>3559.9</v>
       </c>
       <c r="B96" s="3">
-        <v>54.71</v>
+        <v>53.98</v>
       </c>
       <c r="C96" s="3">
-        <v>22.31</v>
+        <v>23.14</v>
       </c>
       <c r="D96" s="3">
-        <v>3134.7</v>
+        <v>3110.3</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
@@ -3595,16 +3602,16 @@
     </row>
     <row r="97" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
-        <v>3642.1</v>
+        <v>3601.7</v>
       </c>
       <c r="B97" s="3">
-        <v>54.84</v>
+        <v>54.71</v>
       </c>
       <c r="C97" s="3">
-        <v>22.15</v>
+        <v>22.31</v>
       </c>
       <c r="D97" s="3">
-        <v>3158</v>
+        <v>3134.7</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
@@ -3629,16 +3636,16 @@
     </row>
     <row r="98" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
-        <v>3682.4</v>
+        <v>3642.1</v>
       </c>
       <c r="B98" s="3">
-        <v>55.13</v>
+        <v>54.84</v>
       </c>
       <c r="C98" s="3">
-        <v>22.24</v>
+        <v>22.15</v>
       </c>
       <c r="D98" s="3">
-        <v>3181.1</v>
+        <v>3158</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
@@ -3663,16 +3670,16 @@
     </row>
     <row r="99" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
-        <v>3722.9</v>
+        <v>3682.4</v>
       </c>
       <c r="B99" s="3">
-        <v>53.47</v>
+        <v>55.13</v>
       </c>
       <c r="C99" s="3">
-        <v>22.04</v>
+        <v>22.24</v>
       </c>
       <c r="D99" s="3">
-        <v>3204.7</v>
+        <v>3181.1</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
@@ -3697,16 +3704,16 @@
     </row>
     <row r="100" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
-        <v>3761.8</v>
+        <v>3722.9</v>
       </c>
       <c r="B100" s="3">
-        <v>52.67</v>
+        <v>53.47</v>
       </c>
       <c r="C100" s="3">
         <v>22.04</v>
       </c>
       <c r="D100" s="3">
-        <v>3228.1</v>
+        <v>3204.7</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
@@ -3731,7 +3738,7 @@
     </row>
     <row r="101" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
-        <v>3790</v>
+        <v>3761.8</v>
       </c>
       <c r="B101" s="3">
         <v>52.67</v>
@@ -3740,7 +3747,7 @@
         <v>22.04</v>
       </c>
       <c r="D101" s="3">
-        <v>3245.2</v>
+        <v>3228.1</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
@@ -3763,11 +3770,19 @@
       <c r="W101" s="2"/>
       <c r="X101" s="2"/>
     </row>
-    <row r="102" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="2"/>
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
+    <row r="102" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3">
+        <v>3790</v>
+      </c>
+      <c r="B102" s="3">
+        <v>52.67</v>
+      </c>
+      <c r="C102" s="3">
+        <v>22.04</v>
+      </c>
+      <c r="D102" s="3">
+        <v>3245.2</v>
+      </c>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
@@ -27111,6 +27126,32 @@
       <c r="W999" s="2"/>
       <c r="X999" s="2"/>
     </row>
+    <row r="1000" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1000" s="2"/>
+      <c r="B1000" s="2"/>
+      <c r="C1000" s="2"/>
+      <c r="D1000" s="2"/>
+      <c r="E1000" s="2"/>
+      <c r="F1000" s="2"/>
+      <c r="G1000" s="2"/>
+      <c r="H1000" s="2"/>
+      <c r="I1000" s="2"/>
+      <c r="J1000" s="2"/>
+      <c r="K1000" s="2"/>
+      <c r="L1000" s="2"/>
+      <c r="M1000" s="2"/>
+      <c r="N1000" s="2"/>
+      <c r="O1000" s="2"/>
+      <c r="P1000" s="2"/>
+      <c r="Q1000" s="2"/>
+      <c r="R1000" s="2"/>
+      <c r="S1000" s="2"/>
+      <c r="T1000" s="2"/>
+      <c r="U1000" s="2"/>
+      <c r="V1000" s="2"/>
+      <c r="W1000" s="2"/>
+      <c r="X1000" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>